<commit_message>
Update excel + artiste sur bonne scène
</commit_message>
<xml_diff>
--- a/LineTest.xlsx
+++ b/LineTest.xlsx
@@ -275,7 +275,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -347,7 +347,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G3" s="4" t="n">
         <v>1</v>
@@ -370,7 +370,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4" s="4" t="n">
         <v>0</v>
@@ -393,7 +393,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G5" s="4" t="n">
         <v>0</v>
@@ -416,7 +416,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G6" s="4" t="n">
         <v>1</v>
@@ -439,7 +439,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="4" t="n">
         <v>0</v>
@@ -842,7 +842,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -887,7 +887,7 @@
       <c r="E2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -896,7 +896,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>90000</v>
@@ -907,7 +907,7 @@
       <c r="E3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -916,7 +916,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>100000</v>
@@ -927,7 +927,7 @@
       <c r="E4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -936,7 +936,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>120000</v>
@@ -947,7 +947,7 @@
       <c r="E5" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>4</v>
       </c>
     </row>
@@ -956,7 +956,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="n">
         <v>130000</v>
@@ -967,7 +967,7 @@
       <c r="E6" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>5</v>
       </c>
     </row>
@@ -976,7 +976,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>150000</v>
@@ -987,7 +987,7 @@
       <c r="E7" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug roll infini une fois qu'un joueur à passer pendant les enchères ?!? (2 joueurs, budget ok, affichage nom du joueur bug)
Error : {'name': 'Joueur 1', 'budget': 810000, 'score': 0, 'ordi': False, 'inventory': {'artists': ['Upsilone'], 'scenes': ['La Clairière', 'La madrague']}} ne peut pas acheter Michelle car il n'a plus assez d'écocups.
</commit_message>
<xml_diff>
--- a/LineTest.xlsx
+++ b/LineTest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Artistes" sheetId="1" state="visible" r:id="rId2"/>
@@ -274,8 +274,8 @@
   </sheetPr>
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -350,7 +350,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,7 +373,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,7 +841,7 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MAJ Rentabilité Bug roll infini while player passe in auction (2p, budget ok, affichage nom du joueur bug)
Error : {'name': 'Joueur 1', 'budget': 810000, 'score': 0, 'ordi': False, 'inventory': {'artists': ['Upsilone'], 'scenes': ['La Clairière', 'La madrague']}} ne peut pas acheter Michelle car il n'a plus assez d'écocups.
</commit_message>
<xml_diff>
--- a/LineTest.xlsx
+++ b/LineTest.xlsx
@@ -176,12 +176,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -218,7 +224,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,6 +242,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,7 +289,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -326,7 +340,7 @@
       <c r="F2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -349,7 +363,7 @@
       <c r="F3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="n">
+      <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -372,7 +386,7 @@
       <c r="F4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -395,7 +409,7 @@
       <c r="F5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="4" t="n">
+      <c r="G5" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -418,7 +432,7 @@
       <c r="F6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="4" t="n">
+      <c r="G6" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -441,7 +455,7 @@
       <c r="F7" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="4" t="n">
+      <c r="G7" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -852,10 +866,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1118,14 +1132,14 @@
       <c r="E25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1171,7 +1185,7 @@
       <c r="B2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="10" t="n">
         <f aca="false">COUNTIF(Artistes!E2:E49,0)</f>
         <v>0</v>
       </c>
@@ -1206,7 +1220,7 @@
         <f aca="false">COUNTIF(Artistes!E2:E49,2)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="8" t="n">
+      <c r="E4" s="10" t="n">
         <f aca="false">COUNTIF(Artistes!G2:G49,0)</f>
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
MAJ scoring (AllScenesStyle (à tester + variousstyles à coder)
Bug roll infini while player passe in auction (2p, budget ok, affichage nom du joueur bug)
</commit_message>
<xml_diff>
--- a/LineTest.xlsx
+++ b/LineTest.xlsx
@@ -224,7 +224,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -239,10 +239,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -289,7 +285,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -332,7 +328,7 @@
         <v>80000</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>2</v>
@@ -340,7 +336,7 @@
       <c r="F2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="n">
+      <c r="G2" s="4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -355,7 +351,7 @@
         <v>10000</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>3</v>
@@ -363,7 +359,7 @@
       <c r="F3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -378,7 +374,7 @@
         <v>10000</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>1</v>
@@ -386,7 +382,7 @@
       <c r="F4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -409,7 +405,7 @@
       <c r="F5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -424,7 +420,7 @@
         <v>50000</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>4</v>
@@ -432,7 +428,7 @@
       <c r="F6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -447,7 +443,7 @@
         <v>1000000</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>3</v>
@@ -455,7 +451,7 @@
       <c r="F7" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -856,7 +852,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -866,10 +862,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1132,14 +1128,14 @@
       <c r="E25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1185,7 +1181,7 @@
       <c r="B2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="9" t="n">
         <f aca="false">COUNTIF(Artistes!E2:E49,0)</f>
         <v>0</v>
       </c>
@@ -1220,7 +1216,7 @@
         <f aca="false">COUNTIF(Artistes!E2:E49,2)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="E4" s="9" t="n">
         <f aca="false">COUNTIF(Artistes!G2:G49,0)</f>
         <v>3</v>
       </c>

</xml_diff>